<commit_message>
Create page input spendding
</commit_message>
<xml_diff>
--- a/0. Học lớp_daily note.xlsx
+++ b/0. Học lớp_daily note.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>Buổi</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Là ngôn ngữ tạo webpage. Cấu trúc từ các thẻ và các liên kết siêu văn bản</t>
+  </si>
+  <si>
+    <t>Mục tiêu là các thẻ cơ bản để tạo ra 1 trang web html cơ bản</t>
+  </si>
+  <si>
+    <t>Ctrl + / : Phím tắt dùng để cmt code</t>
   </si>
 </sst>
 </file>
@@ -1099,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1127,12 +1133,16 @@
       <c r="B5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="D5" s="8"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="13"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
js to validate form
</commit_message>
<xml_diff>
--- a/0. Học lớp_daily note.xlsx
+++ b/0. Học lớp_daily note.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="24.4" sheetId="1" r:id="rId1"/>
-    <sheet name="6.5" sheetId="2" r:id="rId2"/>
+    <sheet name="6.5+8.5" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>Buổi</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>Ctrl + / : Phím tắt dùng để cmt code</t>
+  </si>
+  <si>
+    <t>CSS - HTML: Cách nắm đầu các thẻ đẻ chỉnh css</t>
+  </si>
+  <si>
+    <t>JS - hTML: Cách nắm đầu các thẻ theo object để chỉnh sửa theo js</t>
   </si>
 </sst>
 </file>
@@ -680,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1105,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1147,12 +1153,16 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="13"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="13"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
code gym bai thuc hanh
</commit_message>
<xml_diff>
--- a/0. Học lớp_daily note.xlsx
+++ b/0. Học lớp_daily note.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
   <si>
     <t>Buổi</t>
   </si>
@@ -264,6 +264,15 @@
   </si>
   <si>
     <t>ke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form mà có action cả ô input </t>
+  </si>
+  <si>
+    <t>+ Action nó là hành động gửi tới trang đó</t>
+  </si>
+  <si>
+    <t>+ input là value của cái attribute name VD ?q=MTP</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1173,7 @@
   <dimension ref="B4:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1229,12 +1238,16 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="13"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="13"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="16" t="s">
         <v>69</v>
@@ -1245,7 +1258,9 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="13"/>
-      <c r="C12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>82</v>
+      </c>
       <c r="D12" s="8"/>
       <c r="E12" s="16" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
test Js and form, table, githubbai giang
</commit_message>
<xml_diff>
--- a/0. Học lớp_daily note.xlsx
+++ b/0. Học lớp_daily note.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="24.4" sheetId="1" r:id="rId1"/>
     <sheet name="6.5+8.5" sheetId="2" r:id="rId2"/>
+    <sheet name="13.5" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="286">
   <si>
     <t>Buổi</t>
   </si>
@@ -273,13 +274,1485 @@
   </si>
   <si>
     <t>+ input là value của cái attribute name VD ?q=MTP</t>
+  </si>
+  <si>
+    <t>cách thực thi của JS</t>
+  </si>
+  <si>
+    <t>Nhúng đc JS vào web</t>
+  </si>
+  <si>
+    <t>Cách sử dụng cú pháp JS</t>
+  </si>
+  <si>
+    <t>Sử dụng hàm nhập, hàm xuất của JS</t>
+  </si>
+  <si>
+    <t>Sử dụng chú thích trong JS</t>
+  </si>
+  <si>
+    <t>Debug với ứng dụng JS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Câu hỏi rất hay! Chúng ta sẽ cùng hiểu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"tư duy của ngôn ngữ JavaScript"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> là gì – và nó khác gì so với những ngôn ngữ như </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Java</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hay </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Python</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>✅ "Tư duy của một ngôn ngữ lập trình" là gì?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hiểu đơn giản, đó là </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cách mà ngôn ngữ ấy tư duy, tổ chức và xử lý dữ liệu, hành vi, logic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>⏩ Mỗi ngôn ngữ có "cách nghĩ" khác nhau về:</t>
+  </si>
+  <si>
+    <t>Biến (variable), kiểu dữ liệu</t>
+  </si>
+  <si>
+    <t>Hàm (function), đối tượng (object)</t>
+  </si>
+  <si>
+    <t>Cách xử lý bất đồng bộ (async)</t>
+  </si>
+  <si>
+    <t>Cách thao tác với giao diện (DOM)</t>
+  </si>
+  <si>
+    <t>✅ Tư duy của ngôn ngữ JavaScript là gì?</t>
+  </si>
+  <si>
+    <t>1. 🔁 Hướng sự kiện &amp; tương tác người dùng</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JavaScript là ngôn ngữ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"sống trong trình duyệt"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, tư duy của nó xoay quanh:</t>
+    </r>
+  </si>
+  <si>
+    <t>Người dùng click gì?</t>
+  </si>
+  <si>
+    <t>Gõ gì vào input?</t>
+  </si>
+  <si>
+    <t>Trang tải tới đâu?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">📌 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ví dụ:</t>
+    </r>
+  </si>
+  <si>
+    <t>document.getElementById("btn").onclick = function() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  alert("Bạn vừa bấm nút!");</t>
+  </si>
+  <si>
+    <t>};</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">→ Tư duy JavaScript là: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"đợi người dùng làm gì đó rồi phản hồi lại"</t>
+    </r>
+  </si>
+  <si>
+    <t>2. ⏱ Bất đồng bộ (asynchronous)</t>
+  </si>
+  <si>
+    <t>JavaScript không "đợi" mã chạy xong mới tiếp tục.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nó dùng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>callback</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>Promise</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>async/await</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> để xử lý các hành động như gọi API.</t>
+    </r>
+  </si>
+  <si>
+    <t>async function getData() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  let response = await fetch("https://api.example.com");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  let data = await response.json();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log(data);</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">→ Tư duy: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Cứ chạy tiếp, việc nào cần đợi thì xử lý riêng"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – không giống Java truyền thống.</t>
+    </r>
+  </si>
+  <si>
+    <t>3. 🧱 Function là “công dân hạng nhất”</t>
+  </si>
+  <si>
+    <t>Hàm trong JavaScript có thể gán vào biến, truyền làm tham số, trả về hàm khác.</t>
+  </si>
+  <si>
+    <t>function greet(name) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  return function() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    console.log("Hello " + name);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  };</t>
+  </si>
+  <si>
+    <t>let sayHi = greet("Trung");</t>
+  </si>
+  <si>
+    <t>sayHi(); // in ra: Hello Trung</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">→ Tư duy: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Hàm cũng là dữ liệu"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – rất linh hoạt (khác Java – mọi thứ bị ràng buộc kiểu dữ liệu).</t>
+    </r>
+  </si>
+  <si>
+    <t>4. 🧰 Không bắt ép kiểu dữ liệu (dynamic typing)</t>
+  </si>
+  <si>
+    <r>
+      <t>Bạn không cần khai báo kiểu biến (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>...), JavaScript đoán giúp bạn.</t>
+    </r>
+  </si>
+  <si>
+    <t>let x = 5;</t>
+  </si>
+  <si>
+    <t>x = "Hello"; // vẫn hợp lệ</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">→ Tư duy: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Linh hoạt, không ràng buộc"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> → phù hợp cho phát triển nhanh, nhưng dễ lỗi.</t>
+    </r>
+  </si>
+  <si>
+    <t>🆚 So sánh với các ngôn ngữ khác:</t>
+  </si>
+  <si>
+    <t>Tư duy</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Kiểu dữ liệu</t>
+  </si>
+  <si>
+    <t>Không cần khai báo rõ ràng</t>
+  </si>
+  <si>
+    <t>Bắt buộc khai báo</t>
+  </si>
+  <si>
+    <t>Không bắt buộc</t>
+  </si>
+  <si>
+    <t>Bất đồng bộ</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Có </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>async/await</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Promise</t>
+    </r>
+  </si>
+  <si>
+    <t>Phức tạp hơn</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dùng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>asyncio</t>
+    </r>
+  </si>
+  <si>
+    <t>Tương tác người dùng</t>
+  </si>
+  <si>
+    <t>Tốt, có sẵn DOM API</t>
+  </si>
+  <si>
+    <t>Không có (Java chạy trên server/app)</t>
+  </si>
+  <si>
+    <t>Không có trên web frontend</t>
+  </si>
+  <si>
+    <t>Hàm là dữ liệu</t>
+  </si>
+  <si>
+    <t>Có</t>
+  </si>
+  <si>
+    <t>Không (truyền qua interface)</t>
+  </si>
+  <si>
+    <t>Mục tiêu chính</t>
+  </si>
+  <si>
+    <t>Web frontend, backend</t>
+  </si>
+  <si>
+    <t>App lớn, hệ thống</t>
+  </si>
+  <si>
+    <t>Script, khoa học dữ liệu</t>
+  </si>
+  <si>
+    <t>🎯 Kết luận:</t>
+  </si>
+  <si>
+    <r>
+      <t>Tư duy của JavaScript</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> là: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>linh hoạt – hướng sự kiện – không ràng buộc – xử lý bất đồng bộ – lấy người dùng làm trung tâm.</t>
+    </r>
+  </si>
+  <si>
+    <t>Để giỏi JS, bạn cần quen với:</t>
+  </si>
+  <si>
+    <t>Viết hàm gọn gàng</t>
+  </si>
+  <si>
+    <t>Làm việc với DOM</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hiểu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>callback</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>Promise</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>async/await</t>
+    </r>
+  </si>
+  <si>
+    <t>Bạn có muốn mình thiết kế một loạt ví dụ từ dễ đến nâng cao để luyện “tư duy JavaScript” không?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tuyệt! Dưới đây là một </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lộ trình các ví dụ JavaScript từ dễ đến nâng cao</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, giúp bạn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>luyện tư duy lập trình JavaScript</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> từng bước – từ cơ bản đến ứng dụng thực tế.</t>
+    </r>
+  </si>
+  <si>
+    <t>🟢 Cấp độ 1: Cơ bản – Biến, hàm, điều kiện</t>
+  </si>
+  <si>
+    <t>🧪 Bài 1: Kiểm tra số chẵn lẻ</t>
+  </si>
+  <si>
+    <t>function isEven(number) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  if (number % 2 === 0) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    console.log("Số chẵn");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  } else {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    console.log("Số lẻ");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }</t>
+  </si>
+  <si>
+    <t>isEven(5);</t>
+  </si>
+  <si>
+    <t>🧪 Bài 2: Tính tổng các số từ 1 đến n</t>
+  </si>
+  <si>
+    <t>function sumToN(n) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  let total = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  for (let i = 1; i &lt;= n; i++) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    total += i;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log("Tổng:", total);</t>
+  </si>
+  <si>
+    <t>sumToN(10);</t>
+  </si>
+  <si>
+    <t>🟡 Cấp độ 2: Tương tác với HTML – DOM + Sự kiện</t>
+  </si>
+  <si>
+    <t>🧪 Bài 3: Bấm nút hiển thị lời chào</t>
+  </si>
+  <si>
+    <t>HTML:</t>
+  </si>
+  <si>
+    <t>&lt;button onclick="sayHello()"&gt;Bấm tôi&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>JS:</t>
+  </si>
+  <si>
+    <t>function sayHello() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  alert("Xin chào bạn!");</t>
+  </si>
+  <si>
+    <t>🧪 Bài 4: Đổi màu nền khi click</t>
+  </si>
+  <si>
+    <t>&lt;button onclick="changeColor()"&gt;Đổi màu&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>function changeColor() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  document.body.style.backgroundColor = "lightblue";</t>
+  </si>
+  <si>
+    <t>🟠 Cấp độ 3: Xử lý dữ liệu + form</t>
+  </si>
+  <si>
+    <t>🧪 Bài 5: Lấy dữ liệu từ input</t>
+  </si>
+  <si>
+    <t>&lt;input type="text" id="nameInput" placeholder="Nhập tên"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button onclick="greetUser()"&gt;Chào&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>function greetUser() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  const name = document.getElementById("nameInput").value;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  alert("Xin chào " + name + "!");</t>
+  </si>
+  <si>
+    <t>🧪 Bài 6: Kiểm tra dữ liệu form (simple validation)</t>
+  </si>
+  <si>
+    <t>&lt;input type="email" id="emailInput" placeholder="Email"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button onclick="validateEmail()"&gt;Gửi&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>function validateEmail() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  const email = document.getElementById("emailInput").value;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  if (email.includes("@")) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    alert("Email hợp lệ!");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    alert("Email không hợp lệ!");</t>
+  </si>
+  <si>
+    <t>🔵 Cấp độ 4: Tư duy bất đồng bộ – async/await</t>
+  </si>
+  <si>
+    <t>🧪 Bài 7: Gọi API giả lập</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  let response = await fetch("https://jsonplaceholder.typicode.com/posts/1");</t>
+  </si>
+  <si>
+    <t>getData();</t>
+  </si>
+  <si>
+    <t>🔴 Cấp độ 5: Ứng dụng mini – Tạo danh sách việc cần làm (To-Do List)</t>
+  </si>
+  <si>
+    <t>&lt;input type="text" id="todoInput" placeholder="Nhập việc cần làm"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button onclick="addTodo()"&gt;Thêm&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul id="todoList"&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>function addTodo() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  const task = document.getElementById("todoInput").value;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  const li = document.createElement("li");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  li.innerText = task;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  document.getElementById("todoList").appendChild(li);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  document.getElementById("todoInput").value = "";</t>
+  </si>
+  <si>
+    <t>✅ Gợi ý nâng cao tiếp theo:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dùng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>setTimeout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>setInterval</t>
+    </r>
+  </si>
+  <si>
+    <t>Dự án nhỏ: Calculator, Quiz, Thời tiết, Ghi chú</t>
+  </si>
+  <si>
+    <t>Kết nối với backend API (giả lập hoặc thật)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bạn muốn mình đóng gói các ví dụ này thành </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file HTML + JS mẫu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> để bạn mở bằng trình duyệt học thử luôn không?</t>
+    </r>
+  </si>
+  <si>
+    <t>Tạo 1 form input số thực, trả ra kqua là chẵn/lẻ ( có validate input)</t>
+  </si>
+  <si>
+    <t>URL đường dẫn ở method get gửi đi tới server. Sẽ bị giới hạn dữ liệu. Và bị show thông tin</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tuyệt! Dưới đây là danh sách đầy đủ và </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cô đọng nhất</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> các </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> và </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">property thường dùng nhất của </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>document</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> trong JavaScript – dùng để truy cập, thao tác với HTML.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">✅ I. Các method (phương thức) hay dùng của </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>document</t>
+    </r>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>getElementById(id)</t>
+  </si>
+  <si>
+    <t>Tìm 1 phần tử theo ID</t>
+  </si>
+  <si>
+    <t>getElementsByClassName(class)</t>
+  </si>
+  <si>
+    <t>Trả về danh sách phần tử có class</t>
+  </si>
+  <si>
+    <t>getElementsByTagName(tag)</t>
+  </si>
+  <si>
+    <t>Trả về danh sách phần tử theo tên thẻ</t>
+  </si>
+  <si>
+    <t>querySelector(selector)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trả về </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 phần tử đầu tiên</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> theo CSS selector</t>
+    </r>
+  </si>
+  <si>
+    <t>querySelectorAll(selector)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trả về </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NodeList nhiều phần tử</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> theo selector</t>
+    </r>
+  </si>
+  <si>
+    <t>createElement(tag)</t>
+  </si>
+  <si>
+    <t>Tạo một thẻ HTML mới</t>
+  </si>
+  <si>
+    <t>createTextNode(text)</t>
+  </si>
+  <si>
+    <t>Tạo node chứa văn bản</t>
+  </si>
+  <si>
+    <t>write(html)</t>
+  </si>
+  <si>
+    <t>Ghi trực tiếp HTML vào document (hiếm dùng, cẩn thận với nó)</t>
+  </si>
+  <si>
+    <t>addEventListener(type, func)</t>
+  </si>
+  <si>
+    <t>Thêm sự kiện cho phần tử</t>
+  </si>
+  <si>
+    <t>📌 Ví dụ nhanh:</t>
+  </si>
+  <si>
+    <t>document.getElementById("title").innerText = "Xin chào!";</t>
+  </si>
+  <si>
+    <t>document.querySelector(".box").style.color = "red";</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">✅ II. Các property (thuộc tính) thường dùng của </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>document</t>
+    </r>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>document.body</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Truy cập đến phần </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>&lt;body&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> của trang</t>
+    </r>
+  </si>
+  <si>
+    <t>document.head</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Truy cập phần </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>&lt;head&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>document.title</t>
+  </si>
+  <si>
+    <t>Tiêu đề của trang (title trên tab)</t>
+  </si>
+  <si>
+    <t>document.URL</t>
+  </si>
+  <si>
+    <t>URL đầy đủ của trang</t>
+  </si>
+  <si>
+    <t>document.domain</t>
+  </si>
+  <si>
+    <t>Tên domain hiện tại</t>
+  </si>
+  <si>
+    <t>document.cookie</t>
+  </si>
+  <si>
+    <t>Truy cập hoặc thiết lập cookie</t>
+  </si>
+  <si>
+    <t>document.forms</t>
+  </si>
+  <si>
+    <t>Trả về danh sách form</t>
+  </si>
+  <si>
+    <t>document.images</t>
+  </si>
+  <si>
+    <t>Trả về danh sách ảnh</t>
+  </si>
+  <si>
+    <t>document.links</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trả về tất cả thẻ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>&lt;a&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> có </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>href</t>
+    </r>
+  </si>
+  <si>
+    <t>console.log(document.title);       // Lấy tiêu đề tab</t>
+  </si>
+  <si>
+    <t>document.title = "Trang mới";      // Đổi tiêu đề trang</t>
+  </si>
+  <si>
+    <t>console.log(document.URL);         // In URL hiện tại</t>
+  </si>
+  <si>
+    <t>✅ III. Các method nâng cao hoặc ít dùng (bonus)</t>
+  </si>
+  <si>
+    <t>document.execCommand()</t>
+  </si>
+  <si>
+    <t>Dùng cho thao tác chỉnh sửa văn bản (đã lỗi thời)</t>
+  </si>
+  <si>
+    <t>document.createRange()</t>
+  </si>
+  <si>
+    <t>Dùng để chọn đoạn DOM phức tạp</t>
+  </si>
+  <si>
+    <t>document.importNode()</t>
+  </si>
+  <si>
+    <t>Nhập một node từ document khác</t>
+  </si>
+  <si>
+    <t>🎯 Gợi ý học:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ưu tiên: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>getElementById</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>querySelector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>createElement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>addEventListener</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thường kết hợp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>document</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> với </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>event</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>validation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DOM tree traversal</t>
+    </r>
+  </si>
+  <si>
+    <t>Bạn có muốn mình gửi bảng cheat sheet (tóm tắt nhanh) bằng hình ảnh để dễ nhớ không?</t>
+  </si>
+  <si>
+    <t>Hiển thị giá trị vào 1 thẻ h1,p.. Của thẻ html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,8 +1795,57 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,6 +1867,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,7 +1942,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -449,6 +1977,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -458,11 +1992,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -751,7 +2316,7 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="8.21875" style="1" customWidth="1"/>
@@ -760,7 +2325,7 @@
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="33">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -771,8 +2336,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="2:4" ht="27.6">
+      <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -780,36 +2345,36 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
+    <row r="6" spans="2:4">
+      <c r="B6" s="15"/>
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
+    <row r="7" spans="2:4">
+      <c r="B7" s="15"/>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="2:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
+    <row r="8" spans="2:4" ht="27.6">
+      <c r="B8" s="15"/>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
+    <row r="9" spans="2:4">
+      <c r="B9" s="15"/>
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="2:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="13"/>
+    <row r="10" spans="2:4" ht="27.6">
+      <c r="B10" s="15"/>
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
@@ -817,78 +2382,78 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="13"/>
+    <row r="11" spans="2:4">
+      <c r="B11" s="15"/>
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
+    <row r="12" spans="2:4">
+      <c r="B12" s="15"/>
       <c r="C12" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
+    <row r="13" spans="2:4">
+      <c r="B13" s="15"/>
       <c r="C13" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
+    <row r="14" spans="2:4">
+      <c r="B14" s="15"/>
       <c r="C14" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
+    <row r="15" spans="2:4">
+      <c r="B15" s="15"/>
       <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="13"/>
+    <row r="16" spans="2:4">
+      <c r="B16" s="15"/>
       <c r="C16" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="13"/>
+    <row r="17" spans="2:4">
+      <c r="B17" s="15"/>
       <c r="C17" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="13"/>
+    <row r="18" spans="2:4">
+      <c r="B18" s="15"/>
       <c r="C18" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="13"/>
+    <row r="19" spans="2:4">
+      <c r="B19" s="15"/>
       <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="13"/>
+    <row r="20" spans="2:4">
+      <c r="B20" s="15"/>
       <c r="C20" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="2:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="13"/>
+    <row r="21" spans="2:4" ht="27.6">
+      <c r="B21" s="15"/>
       <c r="C21" s="9" t="s">
         <v>22</v>
       </c>
@@ -896,8 +2461,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="B22" s="13"/>
+    <row r="22" spans="2:4" ht="69">
+      <c r="B22" s="15"/>
       <c r="C22" s="9" t="s">
         <v>26</v>
       </c>
@@ -905,36 +2470,36 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="13"/>
+    <row r="23" spans="2:4">
+      <c r="B23" s="15"/>
       <c r="C23" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="2:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="13"/>
+    <row r="24" spans="2:4" ht="27.6">
+      <c r="B24" s="15"/>
       <c r="C24" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="13"/>
+    <row r="25" spans="2:4">
+      <c r="B25" s="15"/>
       <c r="C25" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="13"/>
+    <row r="26" spans="2:4">
+      <c r="B26" s="15"/>
       <c r="C26" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="13"/>
+    <row r="27" spans="2:4">
+      <c r="B27" s="15"/>
       <c r="C27" s="9" t="s">
         <v>30</v>
       </c>
@@ -942,102 +2507,102 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="13"/>
+    <row r="28" spans="2:4" ht="27.6">
+      <c r="B28" s="15"/>
       <c r="C28" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B29" s="13"/>
+    <row r="29" spans="2:4">
+      <c r="B29" s="15"/>
       <c r="C29" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="13"/>
+    <row r="30" spans="2:4">
+      <c r="B30" s="15"/>
       <c r="C30" s="9" t="s">
         <v>34</v>
       </c>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="13"/>
+    <row r="31" spans="2:4">
+      <c r="B31" s="15"/>
       <c r="C31" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="13"/>
+    <row r="32" spans="2:4">
+      <c r="B32" s="15"/>
       <c r="C32" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="13"/>
+    <row r="33" spans="2:4">
+      <c r="B33" s="15"/>
       <c r="C33" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="13"/>
+    <row r="34" spans="2:4">
+      <c r="B34" s="15"/>
       <c r="C34" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="13"/>
+    <row r="35" spans="2:4">
+      <c r="B35" s="15"/>
       <c r="C35" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="13"/>
+    <row r="36" spans="2:4">
+      <c r="B36" s="15"/>
       <c r="C36" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="13"/>
+    <row r="37" spans="2:4">
+      <c r="B37" s="15"/>
       <c r="C37" s="9" t="s">
         <v>41</v>
       </c>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="13"/>
+    <row r="38" spans="2:4">
+      <c r="B38" s="15"/>
       <c r="C38" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="13"/>
+    <row r="39" spans="2:4">
+      <c r="B39" s="15"/>
       <c r="C39" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="13"/>
+    <row r="40" spans="2:4">
+      <c r="B40" s="15"/>
       <c r="C40" s="9"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="14"/>
+    <row r="41" spans="2:4">
+      <c r="B41" s="16"/>
       <c r="C41" s="3"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="2:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="12" t="s">
+    <row r="42" spans="2:4" ht="17.399999999999999" customHeight="1">
+      <c r="B42" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -1047,8 +2612,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B43" s="13"/>
+    <row r="43" spans="2:4" ht="14.4">
+      <c r="B43" s="15"/>
       <c r="C43" s="3" t="s">
         <v>55</v>
       </c>
@@ -1056,8 +2621,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B44" s="13"/>
+    <row r="44" spans="2:4" ht="14.4">
+      <c r="B44" s="15"/>
       <c r="C44" s="3" t="s">
         <v>57</v>
       </c>
@@ -1065,15 +2630,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="14"/>
+    <row r="45" spans="2:4">
+      <c r="B45" s="16"/>
       <c r="C45" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="2:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="12" t="s">
+    <row r="46" spans="2:4" ht="17.399999999999999" customHeight="1">
+      <c r="B46" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -1081,74 +2646,74 @@
       </c>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="13"/>
+    <row r="47" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B47" s="15"/>
       <c r="C47" s="9" t="s">
         <v>47</v>
       </c>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="13"/>
+    <row r="48" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B48" s="15"/>
       <c r="C48" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="13"/>
+    <row r="49" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B49" s="15"/>
       <c r="C49" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="13"/>
+    <row r="50" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B50" s="15"/>
       <c r="C50" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="13"/>
+    <row r="51" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B51" s="15"/>
       <c r="C51" s="9" t="s">
         <v>51</v>
       </c>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="13"/>
+    <row r="52" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B52" s="15"/>
       <c r="C52" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="13"/>
+    <row r="53" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B53" s="15"/>
       <c r="C53" s="9" t="s">
         <v>52</v>
       </c>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="13"/>
+    <row r="54" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B54" s="15"/>
       <c r="C54" s="9" t="s">
         <v>52</v>
       </c>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="13"/>
+    <row r="55" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B55" s="15"/>
       <c r="C55" s="9"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="13"/>
+    <row r="56" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B56" s="15"/>
       <c r="C56" s="9"/>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="14"/>
+    <row r="57" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B57" s="16"/>
       <c r="C57" s="9"/>
       <c r="D57" s="5"/>
     </row>
@@ -1172,11 +2737,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="8.21875" style="1" customWidth="1"/>
@@ -1186,7 +2751,7 @@
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="33">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1197,8 +2762,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="2:6">
+      <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1206,274 +2771,274 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
+    <row r="6" spans="2:6">
+      <c r="B6" s="15"/>
       <c r="C6" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
+    <row r="7" spans="2:6">
+      <c r="B7" s="15"/>
       <c r="C7" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
+    <row r="8" spans="2:6">
+      <c r="B8" s="15"/>
       <c r="C8" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
-      <c r="C9" s="15" t="s">
+    <row r="9" spans="2:6" ht="14.4">
+      <c r="B9" s="15"/>
+      <c r="C9" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="13"/>
+    <row r="10" spans="2:6">
+      <c r="B10" s="15"/>
       <c r="C10" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="13"/>
+    <row r="11" spans="2:6">
+      <c r="B11" s="15"/>
       <c r="C11" s="9" t="s">
         <v>81</v>
       </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="13" t="s">
         <v>69</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
+    <row r="12" spans="2:6">
+      <c r="B12" s="15"/>
       <c r="C12" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="13" t="s">
         <v>70</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
+    <row r="13" spans="2:6">
+      <c r="B13" s="15"/>
       <c r="C13" s="9"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="13" t="s">
         <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
+    <row r="14" spans="2:6">
+      <c r="B14" s="15"/>
       <c r="C14" s="9"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="13" t="s">
         <v>72</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
+    <row r="15" spans="2:6">
+      <c r="B15" s="15"/>
       <c r="C15" s="9"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="13"/>
+    <row r="16" spans="2:6">
+      <c r="B16" s="15"/>
       <c r="C16" s="9"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="13"/>
+    <row r="17" spans="2:6">
+      <c r="B17" s="15"/>
       <c r="C17" s="9"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="13"/>
+    <row r="18" spans="2:6">
+      <c r="B18" s="15"/>
       <c r="C18" s="9"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B19" s="13"/>
+    <row r="19" spans="2:6">
+      <c r="B19" s="15"/>
       <c r="C19" s="3"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B20" s="13"/>
+    <row r="20" spans="2:6" ht="20.399999999999999">
+      <c r="B20" s="15"/>
       <c r="C20" s="9"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="13" t="s">
         <v>78</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="13"/>
+    <row r="21" spans="2:6">
+      <c r="B21" s="15"/>
       <c r="C21" s="9"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="13"/>
+    <row r="22" spans="2:6">
+      <c r="B22" s="15"/>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="13"/>
+    <row r="23" spans="2:6">
+      <c r="B23" s="15"/>
       <c r="C23" s="9"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="13"/>
+    <row r="24" spans="2:6">
+      <c r="B24" s="15"/>
       <c r="C24" s="9"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="13"/>
+    <row r="25" spans="2:6">
+      <c r="B25" s="15"/>
       <c r="C25" s="9"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="13"/>
+    <row r="26" spans="2:6">
+      <c r="B26" s="15"/>
       <c r="C26" s="9"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="13"/>
+    <row r="27" spans="2:6">
+      <c r="B27" s="15"/>
       <c r="C27" s="9"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="13"/>
+    <row r="28" spans="2:6">
+      <c r="B28" s="15"/>
       <c r="C28" s="9"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="13"/>
+    <row r="29" spans="2:6">
+      <c r="B29" s="15"/>
       <c r="C29" s="9"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="13"/>
+    <row r="30" spans="2:6">
+      <c r="B30" s="15"/>
       <c r="C30" s="9"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="13"/>
+    <row r="31" spans="2:6">
+      <c r="B31" s="15"/>
       <c r="C31" s="9"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="13"/>
+    <row r="32" spans="2:6">
+      <c r="B32" s="15"/>
       <c r="C32" s="9"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="13"/>
+    <row r="33" spans="2:4">
+      <c r="B33" s="15"/>
       <c r="C33" s="9"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="13"/>
+    <row r="34" spans="2:4">
+      <c r="B34" s="15"/>
       <c r="C34" s="9"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="13"/>
+    <row r="35" spans="2:4">
+      <c r="B35" s="15"/>
       <c r="C35" s="9"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="13"/>
+    <row r="36" spans="2:4">
+      <c r="B36" s="15"/>
       <c r="C36" s="9"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="13"/>
+    <row r="37" spans="2:4">
+      <c r="B37" s="15"/>
       <c r="C37" s="9"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="13"/>
+    <row r="38" spans="2:4">
+      <c r="B38" s="15"/>
       <c r="C38" s="9"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="13"/>
+    <row r="39" spans="2:4">
+      <c r="B39" s="15"/>
       <c r="C39" s="9"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="13"/>
+    <row r="40" spans="2:4">
+      <c r="B40" s="15"/>
       <c r="C40" s="9"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="14"/>
+    <row r="41" spans="2:4">
+      <c r="B41" s="16"/>
       <c r="C41" s="3"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="2:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="12" t="s">
+    <row r="42" spans="2:4" ht="17.399999999999999" customHeight="1">
+      <c r="B42" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="11"/>
     </row>
-    <row r="43" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B43" s="13"/>
+    <row r="43" spans="2:4" ht="14.4">
+      <c r="B43" s="15"/>
       <c r="C43" s="3"/>
       <c r="D43" s="11"/>
     </row>
-    <row r="44" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B44" s="13"/>
+    <row r="44" spans="2:4" ht="14.4">
+      <c r="B44" s="15"/>
       <c r="C44" s="3"/>
       <c r="D44" s="11"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="14"/>
+    <row r="45" spans="2:4">
+      <c r="B45" s="16"/>
       <c r="C45" s="3"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="12" t="s">
+    <row r="46" spans="2:4">
+      <c r="B46" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -1481,8 +3046,8 @@
       </c>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="2:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="13"/>
+    <row r="47" spans="2:4" ht="31.2" customHeight="1">
+      <c r="B47" s="15"/>
       <c r="C47" s="9" t="s">
         <v>60</v>
       </c>
@@ -1490,55 +3055,55 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="13"/>
+    <row r="48" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B48" s="15"/>
       <c r="C48" s="9" t="s">
         <v>61</v>
       </c>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="13"/>
+    <row r="49" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B49" s="15"/>
       <c r="C49" s="9"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="13"/>
+    <row r="50" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B50" s="15"/>
       <c r="C50" s="9"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="13"/>
+    <row r="51" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B51" s="15"/>
       <c r="C51" s="9"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="13"/>
+    <row r="52" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B52" s="15"/>
       <c r="C52" s="3"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="13"/>
+    <row r="53" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B53" s="15"/>
       <c r="C53" s="9"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="13"/>
+    <row r="54" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B54" s="15"/>
       <c r="C54" s="9"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="13"/>
+    <row r="55" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B55" s="15"/>
       <c r="C55" s="9"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="13"/>
+    <row r="56" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B56" s="15"/>
       <c r="C56" s="9"/>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="14"/>
+    <row r="57" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B57" s="16"/>
       <c r="C57" s="9"/>
       <c r="D57" s="5"/>
     </row>
@@ -1554,4 +3119,1965 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:H246"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="8.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="84.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:5" ht="33">
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="30" customHeight="1">
+      <c r="B5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="15"/>
+      <c r="C6" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="15"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="15"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="2:5" ht="14.4">
+      <c r="B9" s="15"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="15"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="15"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="15"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="15"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="15"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="15"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="15"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="15"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="15"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="15"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="15"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="15"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="15"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="15"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="15"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="15"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="15"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="15"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="15"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="15"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="15"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="15"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="15"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="15"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="15"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="15"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="15"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="15"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="15"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="15"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="15"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="16"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="2:4" ht="17.399999999999999" customHeight="1">
+      <c r="B42" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="2:4" ht="14.4">
+      <c r="B43" s="15"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="2:4" ht="14.4">
+      <c r="B44" s="15"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" s="16"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="B46" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47" s="15"/>
+      <c r="C47" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="2:4" ht="13.8" customHeight="1">
+      <c r="B48" s="15"/>
+      <c r="C48" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" spans="2:8" ht="13.8" customHeight="1">
+      <c r="B49" s="15"/>
+      <c r="C49" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="5"/>
+    </row>
+    <row r="50" spans="2:8" ht="13.8" customHeight="1">
+      <c r="B50" s="15"/>
+      <c r="C50" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="2:8" ht="13.8" customHeight="1">
+      <c r="B51" s="15"/>
+      <c r="C51" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" spans="2:8" ht="13.8" customHeight="1">
+      <c r="B52" s="15"/>
+      <c r="C52" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="2:8" ht="13.8" customHeight="1">
+      <c r="B53" s="15"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="2:8" ht="13.8" customHeight="1">
+      <c r="B54" s="15"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="2:8" ht="13.8" customHeight="1">
+      <c r="B55" s="15"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="2:8" ht="13.8" customHeight="1">
+      <c r="B56" s="15"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="2:8" ht="13.8" customHeight="1">
+      <c r="B57" s="16"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="5"/>
+    </row>
+    <row r="60" spans="2:8" ht="14.4">
+      <c r="C60" t="s">
+        <v>89</v>
+      </c>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60"/>
+      <c r="H60" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="14.4">
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="H61"/>
+    </row>
+    <row r="62" spans="2:8" ht="14.4">
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="H62"/>
+    </row>
+    <row r="63" spans="2:8" ht="14.4">
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="H63"/>
+    </row>
+    <row r="64" spans="2:8" ht="23.4">
+      <c r="C64" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="H64" s="17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" ht="14.4">
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="H65"/>
+    </row>
+    <row r="66" spans="3:8" ht="18">
+      <c r="C66" t="s">
+        <v>91</v>
+      </c>
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="H66" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" ht="14.4">
+      <c r="C67"/>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="H67"/>
+    </row>
+    <row r="68" spans="3:8" ht="14.4">
+      <c r="C68" t="s">
+        <v>92</v>
+      </c>
+      <c r="D68"/>
+      <c r="E68"/>
+      <c r="F68"/>
+      <c r="H68" s="21" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" ht="14.4">
+      <c r="C69" s="18"/>
+      <c r="D69"/>
+      <c r="E69"/>
+      <c r="F69"/>
+      <c r="H69" s="21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" ht="14.4">
+      <c r="C70" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D70"/>
+      <c r="E70"/>
+      <c r="F70"/>
+      <c r="H70" s="21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" ht="14.4">
+      <c r="C71" s="18"/>
+      <c r="D71"/>
+      <c r="E71"/>
+      <c r="F71"/>
+      <c r="H71" s="21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" ht="14.4">
+      <c r="C72" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D72"/>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="H72" s="21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" ht="14.4">
+      <c r="C73" s="18"/>
+      <c r="D73"/>
+      <c r="E73"/>
+      <c r="F73"/>
+      <c r="H73" s="21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" ht="14.4">
+      <c r="C74" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D74"/>
+      <c r="E74"/>
+      <c r="F74"/>
+      <c r="H74" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" ht="14.4">
+      <c r="C75" s="18"/>
+      <c r="D75"/>
+      <c r="E75"/>
+      <c r="F75"/>
+      <c r="H75" s="21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" ht="14.4">
+      <c r="C76" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="H76"/>
+    </row>
+    <row r="77" spans="3:8" ht="18">
+      <c r="C77"/>
+      <c r="D77"/>
+      <c r="E77"/>
+      <c r="F77"/>
+      <c r="H77" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8" ht="14.4">
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="H78"/>
+    </row>
+    <row r="79" spans="3:8" ht="14.4">
+      <c r="C79"/>
+      <c r="D79"/>
+      <c r="E79"/>
+      <c r="F79"/>
+      <c r="H79" s="21" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="80" spans="3:8" ht="23.4">
+      <c r="C80" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D80"/>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="H80" s="21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="81" spans="3:8" ht="14.4">
+      <c r="C81"/>
+      <c r="D81"/>
+      <c r="E81"/>
+      <c r="F81"/>
+      <c r="H81" s="21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="82" spans="3:8" ht="18">
+      <c r="C82" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D82"/>
+      <c r="E82"/>
+      <c r="F82"/>
+      <c r="H82" s="21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="83" spans="3:8" ht="14.4">
+      <c r="C83" s="18"/>
+      <c r="D83"/>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="H83" s="21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="84" spans="3:8" ht="14.4">
+      <c r="C84" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="H84" s="21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="85" spans="3:8" ht="14.4">
+      <c r="C85" s="18"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="H85" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="86" spans="3:8" ht="14.4">
+      <c r="C86" s="18"/>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="H86" s="21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="87" spans="3:8" ht="14.4">
+      <c r="C87" s="20"/>
+      <c r="D87"/>
+      <c r="E87"/>
+      <c r="F87"/>
+      <c r="H87"/>
+    </row>
+    <row r="88" spans="3:8" ht="14.4">
+      <c r="C88" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="H88"/>
+    </row>
+    <row r="89" spans="3:8" ht="14.4">
+      <c r="C89" s="20"/>
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="H89"/>
+    </row>
+    <row r="90" spans="3:8" ht="23.4">
+      <c r="C90" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="H90" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="3:8" ht="14.4">
+      <c r="C91" s="20"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="H91"/>
+    </row>
+    <row r="92" spans="3:8" ht="18">
+      <c r="C92" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92"/>
+      <c r="H92" s="19" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="93" spans="3:8" ht="14.4">
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="H93"/>
+    </row>
+    <row r="94" spans="3:8" ht="14.4">
+      <c r="C94" t="s">
+        <v>103</v>
+      </c>
+      <c r="D94"/>
+      <c r="E94"/>
+      <c r="F94"/>
+      <c r="H94" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="95" spans="3:8" ht="14.4">
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="H95"/>
+    </row>
+    <row r="96" spans="3:8" ht="14.4">
+      <c r="C96" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96"/>
+      <c r="H96" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="97" spans="3:8" ht="14.4">
+      <c r="C97" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D97"/>
+      <c r="E97"/>
+      <c r="F97"/>
+      <c r="H97"/>
+    </row>
+    <row r="98" spans="3:8" ht="14.4">
+      <c r="C98" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D98"/>
+      <c r="E98"/>
+      <c r="F98"/>
+      <c r="H98" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="99" spans="3:8" ht="14.4">
+      <c r="C99"/>
+      <c r="D99"/>
+      <c r="E99"/>
+      <c r="F99"/>
+      <c r="H99"/>
+    </row>
+    <row r="100" spans="3:8" ht="14.4">
+      <c r="C100" t="s">
+        <v>107</v>
+      </c>
+      <c r="D100"/>
+      <c r="E100"/>
+      <c r="F100"/>
+      <c r="H100" s="21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="101" spans="3:8" ht="14.4">
+      <c r="C101"/>
+      <c r="D101"/>
+      <c r="E101"/>
+      <c r="F101"/>
+      <c r="H101" s="21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="102" spans="3:8" ht="14.4">
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102"/>
+      <c r="F102"/>
+      <c r="H102" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="3:8" ht="14.4">
+      <c r="C103"/>
+      <c r="D103"/>
+      <c r="E103"/>
+      <c r="F103"/>
+      <c r="H103"/>
+    </row>
+    <row r="104" spans="3:8" ht="18">
+      <c r="C104" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D104"/>
+      <c r="E104"/>
+      <c r="F104"/>
+      <c r="H104"/>
+    </row>
+    <row r="105" spans="3:8" ht="14.4">
+      <c r="C105" s="18"/>
+      <c r="D105"/>
+      <c r="E105"/>
+      <c r="F105"/>
+      <c r="H105"/>
+    </row>
+    <row r="106" spans="3:8" ht="18">
+      <c r="C106" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D106"/>
+      <c r="E106"/>
+      <c r="F106"/>
+      <c r="H106" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="107" spans="3:8" ht="14.4">
+      <c r="C107" s="18"/>
+      <c r="D107"/>
+      <c r="E107"/>
+      <c r="F107"/>
+      <c r="H107"/>
+    </row>
+    <row r="108" spans="3:8" ht="14.4">
+      <c r="C108" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D108"/>
+      <c r="E108"/>
+      <c r="F108"/>
+      <c r="H108" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="109" spans="3:8" ht="14.4">
+      <c r="C109"/>
+      <c r="D109"/>
+      <c r="E109"/>
+      <c r="F109"/>
+      <c r="H109"/>
+    </row>
+    <row r="110" spans="3:8" ht="14.4">
+      <c r="C110" t="s">
+        <v>103</v>
+      </c>
+      <c r="D110"/>
+      <c r="E110"/>
+      <c r="F110"/>
+      <c r="H110" s="21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="111" spans="3:8" ht="14.4">
+      <c r="C111"/>
+      <c r="D111"/>
+      <c r="E111"/>
+      <c r="F111"/>
+      <c r="H111"/>
+    </row>
+    <row r="112" spans="3:8" ht="14.4">
+      <c r="C112" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D112"/>
+      <c r="E112"/>
+      <c r="F112"/>
+      <c r="H112" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="113" spans="3:8" ht="14.4">
+      <c r="C113" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D113"/>
+      <c r="E113"/>
+      <c r="F113"/>
+      <c r="H113"/>
+    </row>
+    <row r="114" spans="3:8" ht="14.4">
+      <c r="C114" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D114"/>
+      <c r="E114"/>
+      <c r="F114"/>
+      <c r="H114" s="21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="115" spans="3:8" ht="14.4">
+      <c r="C115" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D115"/>
+      <c r="E115"/>
+      <c r="F115"/>
+      <c r="H115" s="21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="116" spans="3:8" ht="14.4">
+      <c r="C116" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D116"/>
+      <c r="E116"/>
+      <c r="F116"/>
+      <c r="H116" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="3:8" ht="14.4">
+      <c r="C117"/>
+      <c r="D117"/>
+      <c r="E117"/>
+      <c r="F117"/>
+      <c r="H117"/>
+    </row>
+    <row r="118" spans="3:8" ht="14.4">
+      <c r="C118" t="s">
+        <v>116</v>
+      </c>
+      <c r="D118"/>
+      <c r="E118"/>
+      <c r="F118"/>
+      <c r="H118"/>
+    </row>
+    <row r="119" spans="3:8" ht="14.4">
+      <c r="C119"/>
+      <c r="D119"/>
+      <c r="E119"/>
+      <c r="F119"/>
+      <c r="H119"/>
+    </row>
+    <row r="120" spans="3:8" ht="23.4">
+      <c r="C120"/>
+      <c r="D120"/>
+      <c r="E120"/>
+      <c r="F120"/>
+      <c r="H120" s="17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="121" spans="3:8" ht="14.4">
+      <c r="C121"/>
+      <c r="D121"/>
+      <c r="E121"/>
+      <c r="F121"/>
+      <c r="H121"/>
+    </row>
+    <row r="122" spans="3:8" ht="18">
+      <c r="C122" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D122"/>
+      <c r="E122"/>
+      <c r="F122"/>
+      <c r="H122" s="19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="123" spans="3:8" ht="14.4">
+      <c r="C123" s="18"/>
+      <c r="D123"/>
+      <c r="E123"/>
+      <c r="F123"/>
+      <c r="H123"/>
+    </row>
+    <row r="124" spans="3:8" ht="14.4">
+      <c r="C124" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D124"/>
+      <c r="E124"/>
+      <c r="F124"/>
+      <c r="H124" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="125" spans="3:8" ht="14.4">
+      <c r="C125"/>
+      <c r="D125"/>
+      <c r="E125"/>
+      <c r="F125"/>
+      <c r="H125"/>
+    </row>
+    <row r="126" spans="3:8" ht="14.4">
+      <c r="C126" t="s">
+        <v>103</v>
+      </c>
+      <c r="D126"/>
+      <c r="E126"/>
+      <c r="F126"/>
+      <c r="H126" s="21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="127" spans="3:8" ht="14.4">
+      <c r="C127"/>
+      <c r="D127"/>
+      <c r="E127"/>
+      <c r="F127"/>
+      <c r="H127" s="21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="128" spans="3:8" ht="14.4">
+      <c r="C128" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D128"/>
+      <c r="E128"/>
+      <c r="F128"/>
+      <c r="H128"/>
+    </row>
+    <row r="129" spans="3:8" ht="14.4">
+      <c r="C129" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D129"/>
+      <c r="E129"/>
+      <c r="F129"/>
+      <c r="H129" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="130" spans="3:8" ht="14.4">
+      <c r="C130" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D130"/>
+      <c r="E130"/>
+      <c r="F130"/>
+      <c r="H130"/>
+    </row>
+    <row r="131" spans="3:8" ht="14.4">
+      <c r="C131" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D131"/>
+      <c r="E131"/>
+      <c r="F131"/>
+      <c r="H131" s="21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="132" spans="3:8" ht="14.4">
+      <c r="C132" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D132"/>
+      <c r="E132"/>
+      <c r="F132"/>
+      <c r="H132" s="21" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="133" spans="3:8" ht="14.4">
+      <c r="C133" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D133"/>
+      <c r="E133"/>
+      <c r="F133"/>
+      <c r="H133" s="21" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="134" spans="3:8" ht="14.4">
+      <c r="C134" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D134"/>
+      <c r="E134"/>
+      <c r="F134"/>
+      <c r="H134" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="135" spans="3:8" ht="14.4">
+      <c r="C135"/>
+      <c r="D135"/>
+      <c r="E135"/>
+      <c r="F135"/>
+      <c r="H135"/>
+    </row>
+    <row r="136" spans="3:8" ht="14.4">
+      <c r="C136" t="s">
+        <v>125</v>
+      </c>
+      <c r="D136"/>
+      <c r="E136"/>
+      <c r="F136"/>
+      <c r="H136"/>
+    </row>
+    <row r="137" spans="3:8" ht="14.4">
+      <c r="C137"/>
+      <c r="D137"/>
+      <c r="E137"/>
+      <c r="F137"/>
+      <c r="H137"/>
+    </row>
+    <row r="138" spans="3:8" ht="18">
+      <c r="C138"/>
+      <c r="D138"/>
+      <c r="E138"/>
+      <c r="F138"/>
+      <c r="H138" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="139" spans="3:8" ht="14.4">
+      <c r="C139"/>
+      <c r="D139"/>
+      <c r="E139"/>
+      <c r="F139"/>
+      <c r="H139"/>
+    </row>
+    <row r="140" spans="3:8" ht="18">
+      <c r="C140" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D140"/>
+      <c r="E140"/>
+      <c r="F140"/>
+      <c r="H140" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="141" spans="3:8" ht="14.4">
+      <c r="C141" s="18"/>
+      <c r="D141"/>
+      <c r="E141"/>
+      <c r="F141"/>
+      <c r="H141"/>
+    </row>
+    <row r="142" spans="3:8" ht="14.4">
+      <c r="C142" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D142"/>
+      <c r="E142"/>
+      <c r="F142"/>
+      <c r="H142" s="21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="143" spans="3:8" ht="14.4">
+      <c r="C143"/>
+      <c r="D143"/>
+      <c r="E143"/>
+      <c r="F143"/>
+      <c r="H143" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="144" spans="3:8" ht="14.4">
+      <c r="C144" t="s">
+        <v>103</v>
+      </c>
+      <c r="D144"/>
+      <c r="E144"/>
+      <c r="F144"/>
+      <c r="H144"/>
+    </row>
+    <row r="145" spans="3:8" ht="14.4">
+      <c r="C145"/>
+      <c r="D145"/>
+      <c r="E145"/>
+      <c r="F145"/>
+      <c r="H145" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="146" spans="3:8" ht="14.4">
+      <c r="C146" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D146"/>
+      <c r="E146"/>
+      <c r="F146"/>
+      <c r="H146"/>
+    </row>
+    <row r="147" spans="3:8" ht="14.4">
+      <c r="C147" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D147"/>
+      <c r="E147"/>
+      <c r="F147"/>
+      <c r="H147" s="21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="148" spans="3:8" ht="14.4">
+      <c r="C148"/>
+      <c r="D148"/>
+      <c r="E148"/>
+      <c r="F148"/>
+      <c r="H148" s="21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="149" spans="3:8" ht="14.4">
+      <c r="C149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D149"/>
+      <c r="E149"/>
+      <c r="F149"/>
+      <c r="H149" s="21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="150" spans="3:8" ht="14.4">
+      <c r="C150"/>
+      <c r="D150"/>
+      <c r="E150"/>
+      <c r="F150"/>
+      <c r="H150" s="21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="151" spans="3:8" ht="14.4">
+      <c r="C151"/>
+      <c r="D151"/>
+      <c r="E151"/>
+      <c r="F151"/>
+      <c r="H151" s="21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="152" spans="3:8" ht="14.4">
+      <c r="C152"/>
+      <c r="D152"/>
+      <c r="E152"/>
+      <c r="F152"/>
+      <c r="H152" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="153" spans="3:8" ht="23.4">
+      <c r="C153" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D153"/>
+      <c r="E153"/>
+      <c r="F153"/>
+      <c r="H153" s="21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="154" spans="3:8" ht="14.4">
+      <c r="C154"/>
+      <c r="D154"/>
+      <c r="E154"/>
+      <c r="F154"/>
+      <c r="H154" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="155" spans="3:8" ht="14.4">
+      <c r="C155" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D155" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="E155" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="F155" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H155"/>
+    </row>
+    <row r="156" spans="3:8" ht="28.8">
+      <c r="C156" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="D156" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E156" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F156" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="H156"/>
+    </row>
+    <row r="157" spans="3:8" ht="27.6">
+      <c r="C157" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D157" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="E157" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F157" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="H157"/>
+    </row>
+    <row r="158" spans="3:8" ht="43.2">
+      <c r="C158" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="D158" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E158" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F158" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="H158" s="17" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="159" spans="3:8" ht="28.8">
+      <c r="C159" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D159" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="E159" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F159" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="H159"/>
+    </row>
+    <row r="160" spans="3:8" ht="43.2">
+      <c r="C160" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D160" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E160" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="F160" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="H160" s="19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="161" spans="3:8" ht="14.4">
+      <c r="C161"/>
+      <c r="D161"/>
+      <c r="E161"/>
+      <c r="F161"/>
+      <c r="H161"/>
+    </row>
+    <row r="162" spans="3:8" ht="14.4">
+      <c r="C162"/>
+      <c r="D162"/>
+      <c r="E162"/>
+      <c r="F162"/>
+      <c r="H162" s="21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="163" spans="3:8" ht="23.4">
+      <c r="C163" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D163"/>
+      <c r="E163"/>
+      <c r="F163"/>
+      <c r="H163" s="21" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="164" spans="3:8" ht="14.4">
+      <c r="C164" s="18"/>
+      <c r="D164"/>
+      <c r="E164"/>
+      <c r="F164"/>
+      <c r="H164" s="21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="165" spans="3:8" ht="14.4">
+      <c r="C165" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="D165"/>
+      <c r="E165"/>
+      <c r="F165"/>
+      <c r="H165" s="21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="166" spans="3:8" ht="14.4">
+      <c r="C166" s="18"/>
+      <c r="D166"/>
+      <c r="E166"/>
+      <c r="F166"/>
+      <c r="H166" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="167" spans="3:8" ht="14.4">
+      <c r="C167" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D167"/>
+      <c r="E167"/>
+      <c r="F167"/>
+      <c r="H167" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="168" spans="3:8" ht="14.4">
+      <c r="C168" s="18"/>
+      <c r="D168"/>
+      <c r="E168"/>
+      <c r="F168"/>
+      <c r="H168"/>
+    </row>
+    <row r="169" spans="3:8" ht="14.4">
+      <c r="C169" s="18"/>
+      <c r="D169"/>
+      <c r="E169"/>
+      <c r="F169"/>
+      <c r="H169"/>
+    </row>
+    <row r="170" spans="3:8" ht="14.4">
+      <c r="C170" s="20"/>
+      <c r="D170"/>
+      <c r="E170"/>
+      <c r="F170"/>
+      <c r="H170"/>
+    </row>
+    <row r="171" spans="3:8" ht="23.4">
+      <c r="C171" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D171"/>
+      <c r="E171"/>
+      <c r="F171"/>
+      <c r="H171" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="172" spans="3:8" ht="14.4">
+      <c r="C172" s="20"/>
+      <c r="D172"/>
+      <c r="E172"/>
+      <c r="F172"/>
+      <c r="H172"/>
+    </row>
+    <row r="173" spans="3:8" ht="14.4">
+      <c r="C173" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D173"/>
+      <c r="E173"/>
+      <c r="F173"/>
+      <c r="H173" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="174" spans="3:8" ht="14.4">
+      <c r="C174" s="20"/>
+      <c r="D174"/>
+      <c r="E174"/>
+      <c r="F174"/>
+      <c r="H174"/>
+    </row>
+    <row r="175" spans="3:8" ht="14.4">
+      <c r="C175" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D175"/>
+      <c r="E175"/>
+      <c r="F175"/>
+      <c r="H175" s="21" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="176" spans="3:8" ht="14.4">
+      <c r="C176"/>
+      <c r="D176"/>
+      <c r="E176"/>
+      <c r="F176"/>
+      <c r="H176" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="177" spans="3:8" ht="14.4">
+      <c r="C177"/>
+      <c r="D177"/>
+      <c r="E177"/>
+      <c r="F177"/>
+      <c r="H177" s="21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="178" spans="3:8" ht="14.4">
+      <c r="C178"/>
+      <c r="D178"/>
+      <c r="E178"/>
+      <c r="F178"/>
+      <c r="H178"/>
+    </row>
+    <row r="179" spans="3:8" ht="14.4">
+      <c r="C179" t="s">
+        <v>161</v>
+      </c>
+      <c r="D179"/>
+      <c r="E179"/>
+      <c r="F179"/>
+      <c r="H179" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="180" spans="3:8" ht="14.4">
+      <c r="H180"/>
+    </row>
+    <row r="181" spans="3:8">
+      <c r="C181" s="26"/>
+      <c r="D181" s="26"/>
+      <c r="E181" s="26"/>
+      <c r="F181" s="26"/>
+      <c r="G181" s="26"/>
+      <c r="H181" s="21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="182" spans="3:8">
+      <c r="G182" s="26"/>
+      <c r="H182" s="21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="183" spans="3:8" ht="14.4">
+      <c r="C183" t="s">
+        <v>226</v>
+      </c>
+      <c r="D183"/>
+      <c r="G183" s="26"/>
+      <c r="H183" s="21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="184" spans="3:8" ht="14.4">
+      <c r="C184"/>
+      <c r="D184"/>
+      <c r="G184" s="26"/>
+      <c r="H184" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="185" spans="3:8" ht="14.4">
+      <c r="C185"/>
+      <c r="D185"/>
+      <c r="G185" s="26"/>
+      <c r="H185" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="186" spans="3:8" ht="14.4">
+      <c r="C186"/>
+      <c r="D186"/>
+      <c r="G186" s="26"/>
+      <c r="H186" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="187" spans="3:8" ht="23.4">
+      <c r="C187" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="D187"/>
+      <c r="G187" s="26"/>
+      <c r="H187" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="188" spans="3:8" ht="14.4">
+      <c r="C188"/>
+      <c r="D188"/>
+      <c r="G188" s="26"/>
+      <c r="H188"/>
+    </row>
+    <row r="189" spans="3:8" ht="14.4">
+      <c r="C189" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="D189" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="G189" s="26"/>
+      <c r="H189"/>
+    </row>
+    <row r="190" spans="3:8" ht="14.4">
+      <c r="C190" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="D190" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="G190" s="26"/>
+      <c r="H190"/>
+    </row>
+    <row r="191" spans="3:8" ht="23.4">
+      <c r="C191" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="D191" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="G191" s="26"/>
+      <c r="H191" s="17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="192" spans="3:8" ht="14.4">
+      <c r="C192" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="D192" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="G192" s="26"/>
+      <c r="H192" s="18"/>
+    </row>
+    <row r="193" spans="3:8" ht="14.4">
+      <c r="C193" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="D193" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="G193" s="26"/>
+      <c r="H193" s="18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="194" spans="3:8" ht="14.4">
+      <c r="C194" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="D194" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="G194" s="26"/>
+      <c r="H194" s="18"/>
+    </row>
+    <row r="195" spans="3:8" ht="14.4">
+      <c r="C195" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="D195" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="G195" s="26"/>
+      <c r="H195" s="18" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="196" spans="3:8" ht="14.4">
+      <c r="C196" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="D196" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="G196" s="26"/>
+      <c r="H196" s="18"/>
+    </row>
+    <row r="197" spans="3:8" ht="28.8">
+      <c r="C197" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="D197" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="G197" s="26"/>
+      <c r="H197" s="18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="198" spans="3:8" ht="14.4">
+      <c r="C198" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="D198" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="G198" s="26"/>
+      <c r="H198"/>
+    </row>
+    <row r="199" spans="3:8" ht="14.4">
+      <c r="C199"/>
+      <c r="D199"/>
+      <c r="G199" s="26"/>
+      <c r="H199"/>
+    </row>
+    <row r="200" spans="3:8" ht="14.4">
+      <c r="C200"/>
+      <c r="D200"/>
+      <c r="G200" s="26"/>
+      <c r="H200"/>
+    </row>
+    <row r="201" spans="3:8" ht="18">
+      <c r="C201" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D201"/>
+      <c r="G201" s="26"/>
+      <c r="H201" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="202" spans="3:8" ht="14.4">
+      <c r="C202"/>
+      <c r="D202"/>
+      <c r="G202" s="26"/>
+    </row>
+    <row r="203" spans="3:8" ht="14.4">
+      <c r="C203" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D203"/>
+      <c r="G203" s="26"/>
+    </row>
+    <row r="204" spans="3:8" ht="14.4">
+      <c r="C204" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="D204"/>
+      <c r="G204" s="26"/>
+    </row>
+    <row r="205" spans="3:8" ht="14.4">
+      <c r="C205"/>
+      <c r="D205"/>
+      <c r="G205" s="26"/>
+    </row>
+    <row r="206" spans="3:8" ht="14.4">
+      <c r="C206"/>
+      <c r="D206"/>
+      <c r="G206" s="26"/>
+    </row>
+    <row r="207" spans="3:8" ht="14.4">
+      <c r="C207"/>
+      <c r="D207"/>
+      <c r="G207" s="26"/>
+    </row>
+    <row r="208" spans="3:8" ht="23.4">
+      <c r="C208" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="D208"/>
+      <c r="G208" s="26"/>
+    </row>
+    <row r="209" spans="3:7" ht="14.4">
+      <c r="C209"/>
+      <c r="D209"/>
+      <c r="G209" s="26"/>
+    </row>
+    <row r="210" spans="3:7" ht="14.4">
+      <c r="C210" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="D210" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="G210" s="26"/>
+    </row>
+    <row r="211" spans="3:7" ht="14.4">
+      <c r="C211" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="D211" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="G211" s="26"/>
+    </row>
+    <row r="212" spans="3:7" ht="14.4">
+      <c r="C212" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="D212" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="G212" s="26"/>
+    </row>
+    <row r="213" spans="3:7" ht="14.4">
+      <c r="C213" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="D213" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="G213" s="26"/>
+    </row>
+    <row r="214" spans="3:7" ht="14.4">
+      <c r="C214" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="D214" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="G214" s="26"/>
+    </row>
+    <row r="215" spans="3:7" ht="14.4">
+      <c r="C215" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="D215" s="29" t="s">
+        <v>262</v>
+      </c>
+      <c r="G215" s="26"/>
+    </row>
+    <row r="216" spans="3:7" ht="14.4">
+      <c r="C216" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="D216" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="G216" s="26"/>
+    </row>
+    <row r="217" spans="3:7" ht="14.4">
+      <c r="C217" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="D217" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="G217" s="26"/>
+    </row>
+    <row r="218" spans="3:7" ht="14.4">
+      <c r="C218" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="D218" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="G218" s="26"/>
+    </row>
+    <row r="219" spans="3:7" ht="14.4">
+      <c r="C219" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="D219" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="G219" s="26"/>
+    </row>
+    <row r="220" spans="3:7" ht="14.4">
+      <c r="C220"/>
+      <c r="D220"/>
+      <c r="G220" s="26"/>
+    </row>
+    <row r="221" spans="3:7" ht="14.4">
+      <c r="C221"/>
+      <c r="D221"/>
+      <c r="G221" s="26"/>
+    </row>
+    <row r="222" spans="3:7" ht="18">
+      <c r="C222" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D222"/>
+      <c r="G222" s="26"/>
+    </row>
+    <row r="223" spans="3:7" ht="14.4">
+      <c r="C223"/>
+      <c r="D223"/>
+      <c r="G223" s="26"/>
+    </row>
+    <row r="224" spans="3:7" ht="14.4">
+      <c r="C224" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="D224"/>
+      <c r="G224" s="26"/>
+    </row>
+    <row r="225" spans="3:4" ht="14.4">
+      <c r="C225" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="D225"/>
+    </row>
+    <row r="226" spans="3:4" ht="14.4">
+      <c r="C226" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="D226"/>
+    </row>
+    <row r="227" spans="3:4" ht="14.4">
+      <c r="C227"/>
+      <c r="D227"/>
+    </row>
+    <row r="228" spans="3:4" ht="14.4">
+      <c r="C228"/>
+      <c r="D228"/>
+    </row>
+    <row r="229" spans="3:4" ht="14.4">
+      <c r="C229"/>
+      <c r="D229"/>
+    </row>
+    <row r="230" spans="3:4" ht="23.4">
+      <c r="C230" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="D230"/>
+    </row>
+    <row r="231" spans="3:4" ht="14.4">
+      <c r="C231"/>
+      <c r="D231"/>
+    </row>
+    <row r="232" spans="3:4" ht="14.4">
+      <c r="C232" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="D232" s="22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="233" spans="3:4" ht="14.4">
+      <c r="C233" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="D233" s="23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="234" spans="3:4" ht="14.4">
+      <c r="C234" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="D234" s="23" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="235" spans="3:4" ht="14.4">
+      <c r="C235" s="27" t="s">
+        <v>279</v>
+      </c>
+      <c r="D235" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="236" spans="3:4" ht="14.4">
+      <c r="C236"/>
+      <c r="D236"/>
+    </row>
+    <row r="237" spans="3:4" ht="14.4">
+      <c r="C237"/>
+      <c r="D237"/>
+    </row>
+    <row r="238" spans="3:4" ht="23.4">
+      <c r="C238" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="D238"/>
+    </row>
+    <row r="239" spans="3:4" ht="14.4">
+      <c r="C239" s="18"/>
+      <c r="D239"/>
+    </row>
+    <row r="240" spans="3:4" ht="14.4">
+      <c r="C240" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="D240"/>
+    </row>
+    <row r="241" spans="3:4" ht="14.4">
+      <c r="C241" s="18"/>
+      <c r="D241"/>
+    </row>
+    <row r="242" spans="3:4" ht="14.4">
+      <c r="C242" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="D242"/>
+    </row>
+    <row r="243" spans="3:4" ht="14.4">
+      <c r="C243"/>
+      <c r="D243"/>
+    </row>
+    <row r="244" spans="3:4" ht="14.4">
+      <c r="C244"/>
+      <c r="D244"/>
+    </row>
+    <row r="245" spans="3:4" ht="14.4">
+      <c r="C245"/>
+      <c r="D245"/>
+    </row>
+    <row r="246" spans="3:4" ht="14.4">
+      <c r="C246" t="s">
+        <v>284</v>
+      </c>
+      <c r="D246"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B5:B41"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B46:B57"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>